<commit_message>
implementing a new idea, useful in long term. building something genereic
</commit_message>
<xml_diff>
--- a/documents/Design doc.xlsx
+++ b/documents/Design doc.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal\Stock market investment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abhijit Patra\OneDrive\projects\Technical\StockMarketAnalyzer\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47EE7BC6-397F-4FEE-8C13-8C62AFA1F0A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1062715-0762-427E-BD54-4B797BF36DEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8BD4D62F-CA13-407D-B30F-E9A78808E7C9}"/>
+    <workbookView xWindow="1116" yWindow="1116" windowWidth="17280" windowHeight="8964" xr2:uid="{8BD4D62F-CA13-407D-B30F-E9A78808E7C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Yearly" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -265,10 +267,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -586,7 +588,7 @@
   <dimension ref="A1:AZ27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:C14"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -664,7 +666,7 @@
       </c>
     </row>
     <row r="4" spans="1:52" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>49</v>
       </c>
       <c r="B4" s="2"/>
@@ -679,83 +681,83 @@
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
-      <c r="N4" s="7">
+      <c r="N4" s="8">
         <v>2020</v>
       </c>
-      <c r="O4" s="7"/>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="7">
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
+      <c r="Q4" s="8">
         <f>N4-1</f>
         <v>2019</v>
       </c>
-      <c r="R4" s="7"/>
-      <c r="S4" s="7"/>
-      <c r="T4" s="7">
+      <c r="R4" s="8"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="8">
         <f t="shared" ref="T4" si="0">Q4-1</f>
         <v>2018</v>
       </c>
-      <c r="U4" s="7"/>
-      <c r="V4" s="7"/>
-      <c r="W4" s="7">
+      <c r="U4" s="8"/>
+      <c r="V4" s="8"/>
+      <c r="W4" s="8">
         <f t="shared" ref="W4" si="1">T4-1</f>
         <v>2017</v>
       </c>
-      <c r="X4" s="7"/>
-      <c r="Y4" s="7"/>
-      <c r="Z4" s="7">
+      <c r="X4" s="8"/>
+      <c r="Y4" s="8"/>
+      <c r="Z4" s="8">
         <f t="shared" ref="Z4" si="2">W4-1</f>
         <v>2016</v>
       </c>
-      <c r="AA4" s="7"/>
-      <c r="AB4" s="7"/>
-      <c r="AC4" s="7">
+      <c r="AA4" s="8"/>
+      <c r="AB4" s="8"/>
+      <c r="AC4" s="8">
         <f t="shared" ref="AC4" si="3">Z4-1</f>
         <v>2015</v>
       </c>
-      <c r="AD4" s="7"/>
-      <c r="AE4" s="7"/>
-      <c r="AF4" s="7">
+      <c r="AD4" s="8"/>
+      <c r="AE4" s="8"/>
+      <c r="AF4" s="8">
         <f t="shared" ref="AF4" si="4">AC4-1</f>
         <v>2014</v>
       </c>
-      <c r="AG4" s="7"/>
-      <c r="AH4" s="7"/>
-      <c r="AI4" s="7">
+      <c r="AG4" s="8"/>
+      <c r="AH4" s="8"/>
+      <c r="AI4" s="8">
         <f t="shared" ref="AI4" si="5">AF4-1</f>
         <v>2013</v>
       </c>
-      <c r="AJ4" s="7"/>
-      <c r="AK4" s="7"/>
-      <c r="AL4" s="7">
+      <c r="AJ4" s="8"/>
+      <c r="AK4" s="8"/>
+      <c r="AL4" s="8">
         <f t="shared" ref="AL4" si="6">AI4-1</f>
         <v>2012</v>
       </c>
-      <c r="AM4" s="7"/>
-      <c r="AN4" s="7"/>
-      <c r="AO4" s="7">
+      <c r="AM4" s="8"/>
+      <c r="AN4" s="8"/>
+      <c r="AO4" s="8">
         <f t="shared" ref="AO4" si="7">AL4-1</f>
         <v>2011</v>
       </c>
-      <c r="AP4" s="7"/>
-      <c r="AQ4" s="7"/>
-      <c r="AR4" s="7">
+      <c r="AP4" s="8"/>
+      <c r="AQ4" s="8"/>
+      <c r="AR4" s="8">
         <f t="shared" ref="AR4" si="8">AO4-1</f>
         <v>2010</v>
       </c>
-      <c r="AS4" s="7"/>
-      <c r="AT4" s="7"/>
-      <c r="AU4" s="7">
+      <c r="AS4" s="8"/>
+      <c r="AT4" s="8"/>
+      <c r="AU4" s="8">
         <f t="shared" ref="AU4" si="9">AR4-1</f>
         <v>2009</v>
       </c>
-      <c r="AV4" s="7"/>
-      <c r="AW4" s="7"/>
-      <c r="AX4" s="7">
+      <c r="AV4" s="8"/>
+      <c r="AW4" s="8"/>
+      <c r="AX4" s="8">
         <f t="shared" ref="AX4" si="10">AU4-1</f>
         <v>2008</v>
       </c>
-      <c r="AY4" s="7"/>
-      <c r="AZ4" s="7"/>
+      <c r="AY4" s="8"/>
+      <c r="AZ4" s="8"/>
     </row>
     <row r="5" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
@@ -1236,11 +1238,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="N4:P4"/>
-    <mergeCell ref="Q4:S4"/>
-    <mergeCell ref="T4:V4"/>
-    <mergeCell ref="W4:Y4"/>
-    <mergeCell ref="AO4:AQ4"/>
     <mergeCell ref="AR4:AT4"/>
     <mergeCell ref="AU4:AW4"/>
     <mergeCell ref="AX4:AZ4"/>
@@ -1249,6 +1246,11 @@
     <mergeCell ref="AF4:AH4"/>
     <mergeCell ref="AI4:AK4"/>
     <mergeCell ref="AL4:AN4"/>
+    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="Q4:S4"/>
+    <mergeCell ref="T4:V4"/>
+    <mergeCell ref="W4:Y4"/>
+    <mergeCell ref="AO4:AQ4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>